<commit_message>
Love on the Rocks
</commit_message>
<xml_diff>
--- a/pieces.xlsx
+++ b/pieces.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Komponente</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
+    <t xml:space="preserve">Anzahl Stationen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gehäuse A</t>
   </si>
   <si>
@@ -65,6 +68,18 @@
   </si>
   <si>
     <t xml:space="preserve">Arduino MKR NB 1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUT 0820 T8CW 04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchse Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUM 0270-02</t>
   </si>
 </sst>
 </file>
@@ -80,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,6 +117,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,12 +162,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,15 +183,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,123 +318,167 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.97"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="80.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="17.13"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>11.99</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <f aca="false">C2*D2</f>
         <v>119.9</v>
       </c>
+      <c r="H2" s="4" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="n">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>793.72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>95.56</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="n">
+      <c r="D4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <f aca="false">C4*D4</f>
         <v>955.6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>86.05</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="n">
+      <c r="D6" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="n">
         <f aca="false">C6*D6</f>
         <v>850</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>7.55</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <f aca="false">C7*D7</f>
+        <v>528.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <f aca="false">C8*D8</f>
+        <v>34.5</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">SUM(E2:E15)</f>
-        <v>2805.27</v>
+        <v>3368.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The King of Assassins
</commit_message>
<xml_diff>
--- a/pieces.xlsx
+++ b/pieces.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t xml:space="preserve">Komponente</t>
   </si>
@@ -74,7 +74,13 @@
     <t xml:space="preserve">Solarpanel</t>
   </si>
   <si>
+    <t xml:space="preserve">https://solarv.de/enjoysolar-Monokristallines-Solarmodul-20W-12V-2-adriges-Solarkabel-1m1mm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Batterie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.conrad.de/de/p/vision-akkus-cp12120d-cp12120d-bleiakku-12-v-12-ah-blei-vlies-agm-b-x-h-x-t-151-x-101-x-98-mm-flachstecker-6-35-mm-w-377145.html?refresh=true</t>
   </si>
   <si>
     <t xml:space="preserve">THERMISTOR</t>
@@ -146,7 +152,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -182,6 +188,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,6 +268,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,7 +409,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -511,6 +532,9 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="2" t="n">
         <v>27.95</v>
       </c>
@@ -524,7 +548,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>59.99</v>
@@ -553,6 +580,8 @@
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://www.reichelt.de/de/de/shop/produkt/einbausteckverbinder_m8_4_pol_kupplung_0_5_m-223096"/>
     <hyperlink ref="B6" r:id="rId2" display="https://www.reichelt.de/de/de/shop/produkt/quicklock-einbaukupplung_-_groesse_12_2_pol-239487"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://solarv.de/enjoysolar-Monokristallines-Solarmodul-20W-12V-2-adriges-Solarkabel-1m1mm"/>
+    <hyperlink ref="B8" r:id="rId4" display="https://www.conrad.de/de/p/vision-akkus-cp12120d-cp12120d-bleiakku-12-v-12-ah-blei-vlies-agm-b-x-h-x-t-151-x-101-x-98-mm-flachstecker-6-35-mm-w-377145.html?refresh=true"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -579,164 +608,164 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <v>3.3</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="G2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="9" t="n">
         <f aca="false">13.8-(0.02*ABS(25-L3))</f>
         <v>13.3</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="K2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="9" t="n">
         <v>2.3</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="9" t="n">
         <f aca="false">6*L2</f>
         <v>13.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9" t="n">
         <v>42.47</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="8" t="n">
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="10" t="n">
         <v>82</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="I3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="K3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="n">
+      <c r="A4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9" t="n">
         <v>3.02</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="8" t="n">
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="n">
         <f aca="false">(H2/2.1-1)*H3</f>
         <v>437.333333333333</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="1" t="n">
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="9" t="n">
         <v>390</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="n">
+      <c r="A5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="n">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="8" t="n">
+      <c r="G6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="10" t="n">
         <f aca="false">2.1*(1+J4/H3)</f>
         <v>12.0878048780488</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>31</v>
+      <c r="A7" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="8" t="n">
+      <c r="A8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="10" t="n">
         <f aca="false">(B2/B5-1)/(1/B9+1/B3)</f>
         <v>5.36446159695818</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8" t="n">
+      <c r="A9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10" t="n">
         <f aca="false">(B2*B3*B4*(1/B5-1/B6))/(B4*(B2/B6-1)-B3*(B2/B5-1))</f>
         <v>10.2436172221012</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="8" t="n">
+      <c r="G10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="10" t="n">
         <f aca="false">1.2*(1+H11/H12)</f>
         <v>17.8333333333333</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="1" t="n">
+      <c r="G11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="9" t="n">
         <v>499</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="1" t="n">
+      <c r="G12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="9" t="n">
         <v>36</v>
       </c>
     </row>

</xml_diff>